<commit_message>
fix BIDMAS mistake in add_to_output function.
</commit_message>
<xml_diff>
--- a/output_table.xlsx
+++ b/output_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,359 +434,467 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Excel table row number</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Excel table row number</t>
+          <t>Question name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Question name</t>
+          <t>Crossbreak subgroup</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Crossbreak subgroup</t>
+          <t>National average for question (%)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>National average for question (%)</t>
+          <t>Proportion for subgroup (%)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Proportion for subgroup (%)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>Significant difference (%)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="n">
+        <v>97</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Retired before the pandemic</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>43.770211919328</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.367092365260114</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-43.40311955406789</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>97</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Retired before the pandemic</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>45-54</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>43.770211919328</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.49356887781973</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-40.27664304150827</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>99</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Currently focusing on education or study</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>9.356530781419</v>
+      </c>
+      <c r="E4" t="n">
+        <v>52.3122273459771</v>
+      </c>
+      <c r="F4" t="n">
+        <v>42.9556965645581</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>111</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Very likely</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>18-24</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="D5" t="n">
         <v>20.0082371014857</v>
       </c>
-      <c r="F2" t="n">
+      <c r="E5" t="n">
         <v>77.76134286736071</v>
       </c>
-      <c r="G2" t="n">
-        <v>-19.23062367281209</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="F5" t="n">
+        <v>57.753105765875</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>115</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Very unlikely</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>18-24</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="D6" t="n">
         <v>58.86715293352231</v>
       </c>
-      <c r="F3" t="n">
+      <c r="E6" t="n">
         <v>4.24767106839781</v>
       </c>
-      <c r="G3" t="n">
-        <v>-58.82467622283833</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
+      <c r="F6" t="n">
+        <v>-54.6194818651245</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>115</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>Very unlikely</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>25-34</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="D7" t="n">
         <v>58.86715293352231</v>
       </c>
-      <c r="F4" t="n">
+      <c r="E7" t="n">
         <v>7.84713647937069</v>
       </c>
-      <c r="G4" t="n">
-        <v>-58.7886815687286</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
+      <c r="F7" t="n">
+        <v>-51.02001645415162</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>117</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>Total Likely:</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>18-24</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="D8" t="n">
         <v>26.477548712461</v>
       </c>
-      <c r="F5" t="n">
+      <c r="E8" t="n">
         <v>88.73009773374551</v>
       </c>
-      <c r="G5" t="n">
-        <v>-25.59024773512355</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
+      <c r="F8" t="n">
+        <v>62.25254902128449</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>118</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>Total Unlikely:</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>18-24</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="D9" t="n">
         <v>64.4043291531944</v>
       </c>
-      <c r="F6" t="n">
+      <c r="E9" t="n">
         <v>5.18587048384209</v>
       </c>
-      <c r="G6" t="n">
-        <v>-64.35247044835597</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
+      <c r="F9" t="n">
+        <v>-59.2184586693523</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>118</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Total Unlikely:</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>25-34</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="D10" t="n">
         <v>64.4043291531944</v>
       </c>
-      <c r="F7" t="n">
+      <c r="E10" t="n">
         <v>10.0463291479188</v>
       </c>
-      <c r="G7" t="n">
-        <v>-64.30386586171521</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
+      <c r="F10" t="n">
+        <v>-54.3580000052756</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>119</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Net:</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>18-24</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="D11" t="n">
         <v>-37.9267804407334</v>
       </c>
-      <c r="F8" t="n">
+      <c r="E11" t="n">
         <v>83.5442272499034</v>
       </c>
-      <c r="G8" t="n">
-        <v>38.76222271323243</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
+      <c r="F11" t="n">
+        <v>121.4710076906368</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>119</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Net:</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>25-34</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="D12" t="n">
         <v>-37.9267804407334</v>
       </c>
-      <c r="F9" t="n">
+      <c r="E12" t="n">
         <v>55.99427110512691</v>
       </c>
-      <c r="G9" t="n">
-        <v>38.48672315178467</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
+      <c r="F12" t="n">
+        <v>93.92105154586031</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>119</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Net:</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>35-44</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="D13" t="n">
         <v>-37.9267804407334</v>
       </c>
-      <c r="F10" t="n">
+      <c r="E13" t="n">
         <v>21.0616633985113</v>
       </c>
-      <c r="G10" t="n">
-        <v>38.13739707471851</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
+      <c r="F13" t="n">
+        <v>58.9884438392447</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>119</v>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Net:</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>65+</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="D14" t="n">
         <v>-37.9267804407334</v>
       </c>
-      <c r="F11" t="n">
+      <c r="E14" t="n">
         <v>-94.85353342083511</v>
       </c>
-      <c r="G11" t="n">
-        <v>36.97824510652504</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
+      <c r="F14" t="n">
+        <v>-56.9267529801017</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>119</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Net:</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>-37.9267804407334</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8.31705680363695</v>
+      </c>
+      <c r="F15" t="n">
+        <v>46.24383724437035</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>1085</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>Somewhat more difficult</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Wales</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="D16" t="n">
         <v>25.7372170148127</v>
       </c>
-      <c r="F12" t="n">
+      <c r="E16" t="n">
         <v>77.6090706348227</v>
       </c>
-      <c r="G12" t="n">
-        <v>-24.96112630846448</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
+      <c r="F16" t="n">
+        <v>51.87185362000999</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>1086</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>Would not have made much difference</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>35-44</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>8.169964514875131</v>
+      </c>
+      <c r="E17" t="n">
+        <v>49.505442985824</v>
+      </c>
+      <c r="F17" t="n">
+        <v>41.33547847094887</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1086</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Would not have made much difference</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>45-54</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="D18" t="n">
         <v>8.169964514875131</v>
       </c>
-      <c r="F13" t="n">
+      <c r="E18" t="n">
         <v>59.1162973399879</v>
       </c>
-      <c r="G13" t="n">
-        <v>-7.578801541475253</v>
+      <c r="F18" t="n">
+        <v>50.94633282511277</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1100</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Significantly more difficult</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>East of England</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>35.4535835172556</v>
+      </c>
+      <c r="E19" t="n">
+        <v>85.3524049118576</v>
+      </c>
+      <c r="F19" t="n">
+        <v>49.898821394602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add user input validation/error handling.
</commit_message>
<xml_diff>
--- a/output_table.xlsx
+++ b/output_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,50 +467,50 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Retired before the pandemic</t>
+          <t>Yes, I have worked remotely in the past</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>18-24</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>43.770211919328</v>
+        <v>30.5790043160841</v>
       </c>
       <c r="E2" t="n">
-        <v>0.367092365260114</v>
+        <v>58.2049452830865</v>
       </c>
       <c r="F2" t="n">
-        <v>-43.40311955406789</v>
+        <v>27.62594096700239</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Retired before the pandemic</t>
+          <t>No, I have never worked remotely</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>45-54</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>43.770211919328</v>
+        <v>68.83138130225859</v>
       </c>
       <c r="E3" t="n">
-        <v>3.49356887781973</v>
+        <v>41.7950547169135</v>
       </c>
       <c r="F3" t="n">
-        <v>-40.27664304150827</v>
+        <v>-27.0363265853451</v>
       </c>
     </row>
     <row r="4">
@@ -519,7 +519,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Currently focusing on education or study</t>
+          <t>Retired before the pandemic</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -528,118 +528,118 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>9.356530781419</v>
+        <v>43.770211919328</v>
       </c>
       <c r="E4" t="n">
-        <v>52.3122273459771</v>
+        <v>0.367092365260114</v>
       </c>
       <c r="F4" t="n">
-        <v>42.9556965645581</v>
+        <v>-43.40311955406789</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Very likely</t>
+          <t>Retired before the pandemic</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>18-24</t>
+          <t>45-54</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>20.0082371014857</v>
+        <v>43.770211919328</v>
       </c>
       <c r="E5" t="n">
-        <v>77.76134286736071</v>
+        <v>3.49356887781973</v>
       </c>
       <c r="F5" t="n">
-        <v>57.753105765875</v>
+        <v>-40.27664304150827</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Very unlikely</t>
+          <t>Retired before the pandemic</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>18-24</t>
+          <t>65+</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>58.86715293352231</v>
+        <v>43.770211919328</v>
       </c>
       <c r="E6" t="n">
-        <v>4.24767106839781</v>
+        <v>81.436589257498</v>
       </c>
       <c r="F6" t="n">
-        <v>-54.6194818651245</v>
+        <v>37.66637733817</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Very unlikely</t>
+          <t>Have a long term medical condition</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>25-34</t>
+          <t>45-54</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>58.86715293352231</v>
+        <v>15.2398770060353</v>
       </c>
       <c r="E7" t="n">
-        <v>7.84713647937069</v>
+        <v>43.9631878632519</v>
       </c>
       <c r="F7" t="n">
-        <v>-51.02001645415162</v>
+        <v>28.7233108572166</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Total Likely:</t>
+          <t>Have a long term medical condition</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>18-24</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>26.477548712461</v>
+        <v>15.2398770060353</v>
       </c>
       <c r="E8" t="n">
-        <v>88.73009773374551</v>
+        <v>48.0137931844539</v>
       </c>
       <c r="F8" t="n">
-        <v>62.25254902128449</v>
+        <v>32.7739161784186</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Total Unlikely:</t>
+          <t>Currently focusing on education or study</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -648,253 +648,2509 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>64.4043291531944</v>
+        <v>9.356530781419</v>
       </c>
       <c r="E9" t="n">
-        <v>5.18587048384209</v>
+        <v>52.3122273459771</v>
       </c>
       <c r="F9" t="n">
-        <v>-59.2184586693523</v>
+        <v>42.9556965645581</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Total Unlikely:</t>
+          <t>Very likely</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>25-34</t>
+          <t>18-24</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>64.4043291531944</v>
+        <v>20.0082371014857</v>
       </c>
       <c r="E10" t="n">
-        <v>10.0463291479188</v>
+        <v>77.76134286736071</v>
       </c>
       <c r="F10" t="n">
-        <v>-54.3580000052756</v>
+        <v>57.753105765875</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Net:</t>
+          <t>Very likely</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>18-24</t>
+          <t>25-34</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>-37.9267804407334</v>
+        <v>20.0082371014857</v>
       </c>
       <c r="E11" t="n">
-        <v>83.5442272499034</v>
+        <v>45.6229015330869</v>
       </c>
       <c r="F11" t="n">
-        <v>121.4710076906368</v>
+        <v>25.6146644316012</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Net:</t>
+          <t>Very unlikely</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>25-34</t>
+          <t>18-24</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-37.9267804407334</v>
+        <v>58.86715293352231</v>
       </c>
       <c r="E12" t="n">
-        <v>55.99427110512691</v>
+        <v>4.24767106839781</v>
       </c>
       <c r="F12" t="n">
-        <v>93.92105154586031</v>
+        <v>-54.6194818651245</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Net:</t>
+          <t>Very unlikely</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>35-44</t>
+          <t>25-34</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-37.9267804407334</v>
+        <v>58.86715293352231</v>
       </c>
       <c r="E13" t="n">
-        <v>21.0616633985113</v>
+        <v>7.84713647937069</v>
       </c>
       <c r="F13" t="n">
-        <v>58.9884438392447</v>
+        <v>-51.02001645415162</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Net:</t>
+          <t>Very unlikely</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>65+</t>
+          <t>35-44</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>-37.9267804407334</v>
+        <v>58.86715293352231</v>
       </c>
       <c r="E14" t="n">
-        <v>-94.85353342083511</v>
+        <v>23.015534772561</v>
       </c>
       <c r="F14" t="n">
-        <v>-56.9267529801017</v>
+        <v>-35.85161816096131</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Net:</t>
+          <t>Very unlikely</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>65+</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>-37.9267804407334</v>
+        <v>58.86715293352231</v>
       </c>
       <c r="E15" t="n">
-        <v>8.31705680363695</v>
+        <v>91.70380552896211</v>
       </c>
       <c r="F15" t="n">
-        <v>46.24383724437035</v>
+        <v>32.83665259543979</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1085</v>
+        <v>119</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Somewhat more difficult</t>
+          <t>Total Likely:</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wales</t>
+          <t>18-24</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>25.7372170148127</v>
+        <v>26.477548712461</v>
       </c>
       <c r="E16" t="n">
-        <v>77.6090706348227</v>
+        <v>88.73009773374551</v>
       </c>
       <c r="F16" t="n">
-        <v>51.87185362000999</v>
+        <v>62.25254902128449</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1086</v>
+        <v>119</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Would not have made much difference</t>
+          <t>Total Likely:</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>35-44</t>
+          <t>25-34</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>8.169964514875131</v>
+        <v>26.477548712461</v>
       </c>
       <c r="E17" t="n">
-        <v>49.505442985824</v>
+        <v>66.0406002530457</v>
       </c>
       <c r="F17" t="n">
-        <v>41.33547847094887</v>
+        <v>39.56305154058469</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1086</v>
+        <v>119</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Would not have made much difference</t>
+          <t>Total Likely:</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>45-54</t>
+          <t>65+</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>8.169964514875131</v>
+        <v>26.477548712461</v>
       </c>
       <c r="E18" t="n">
-        <v>59.1162973399879</v>
+        <v>1.4166814899744</v>
       </c>
       <c r="F18" t="n">
-        <v>50.94633282511277</v>
+        <v>-25.0608672224866</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1100</v>
+        <v>119</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>Total Likely:</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>26.477548712461</v>
+      </c>
+      <c r="E19" t="n">
+        <v>51.6382691741866</v>
+      </c>
+      <c r="F19" t="n">
+        <v>25.1607204617256</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>120</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Total Unlikely:</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>64.4043291531944</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5.18587048384209</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-59.2184586693523</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>120</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Total Unlikely:</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>25-34</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>64.4043291531944</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10.0463291479188</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-54.3580000052756</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>120</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Total Unlikely:</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>35-44</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>64.4043291531944</v>
+      </c>
+      <c r="E22" t="n">
+        <v>29.0614834001557</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-35.3428457530387</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>120</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Total Unlikely:</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>64.4043291531944</v>
+      </c>
+      <c r="E23" t="n">
+        <v>96.2702149108095</v>
+      </c>
+      <c r="F23" t="n">
+        <v>31.86588575761511</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>121</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Net:</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>-37.9267804407334</v>
+      </c>
+      <c r="E24" t="n">
+        <v>83.5442272499034</v>
+      </c>
+      <c r="F24" t="n">
+        <v>121.4710076906368</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>121</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Net:</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>25-34</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>-37.9267804407334</v>
+      </c>
+      <c r="E25" t="n">
+        <v>55.99427110512691</v>
+      </c>
+      <c r="F25" t="n">
+        <v>93.92105154586031</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>121</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Net:</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>35-44</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>-37.9267804407334</v>
+      </c>
+      <c r="E26" t="n">
+        <v>21.0616633985113</v>
+      </c>
+      <c r="F26" t="n">
+        <v>58.9884438392447</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>121</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Net:</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>45-54</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>-37.9267804407334</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-8.30759224471819</v>
+      </c>
+      <c r="F27" t="n">
+        <v>29.61918819601521</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>121</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Net:</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>55-64</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>-37.9267804407334</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-69.2316769605296</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-31.3048965197962</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>121</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Net:</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>-37.9267804407334</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-94.85353342083511</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-56.9267529801017</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>121</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Net:</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>-37.9267804407334</v>
+      </c>
+      <c r="E30" t="n">
+        <v>8.31705680363695</v>
+      </c>
+      <c r="F30" t="n">
+        <v>46.24383724437035</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>137</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>This is a barrier to me finding work</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>28.5748637833026</v>
+      </c>
+      <c r="E31" t="n">
+        <v>62.6738684046556</v>
+      </c>
+      <c r="F31" t="n">
+        <v>34.099004621353</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>138</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>This is not a barrier to me finding work</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>64.6299050780236</v>
+      </c>
+      <c r="E32" t="n">
+        <v>31.2441174241889</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-33.3857876538347</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>143</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>This is a barrier to me finding work</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>38.4367510705753</v>
+      </c>
+      <c r="E33" t="n">
+        <v>71.74330054547259</v>
+      </c>
+      <c r="F33" t="n">
+        <v>33.3065494748973</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>144</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>This is not a barrier to me finding work</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>54.9719841455658</v>
+      </c>
+      <c r="E34" t="n">
+        <v>22.3474456870177</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-32.6245384585481</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>155</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>This is a barrier to me finding work</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>35-44</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>17.809493624109</v>
+      </c>
+      <c r="E35" t="n">
+        <v>47.2926369801579</v>
+      </c>
+      <c r="F35" t="n">
+        <v>29.4831433560489</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>156</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>This is not a barrier to me finding work</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>35-44</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>77.4958272017645</v>
+      </c>
+      <c r="E36" t="n">
+        <v>43.7689564597157</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-33.7268707420488</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>171</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Able to work remotely</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>29.6335464032665</v>
+      </c>
+      <c r="E37" t="n">
+        <v>55.6543110464387</v>
+      </c>
+      <c r="F37" t="n">
+        <v>26.0207646431722</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>171</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Able to work remotely</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>25-34</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>29.6335464032665</v>
+      </c>
+      <c r="E38" t="n">
+        <v>56.0433733830323</v>
+      </c>
+      <c r="F38" t="n">
+        <v>26.4098269797658</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>171</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Able to work remotely</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>35-44</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>29.6335464032665</v>
+      </c>
+      <c r="E39" t="n">
+        <v>58.38383340393351</v>
+      </c>
+      <c r="F39" t="n">
+        <v>28.75028700066701</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>174</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Do more interesting work</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>15.3779744159054</v>
+      </c>
+      <c r="E40" t="n">
+        <v>40.89831998110471</v>
+      </c>
+      <c r="F40" t="n">
+        <v>25.5203455651993</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>175</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>None of the above</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>47.3873282528331</v>
+      </c>
+      <c r="E41" t="n">
+        <v>9.75867649117537</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-37.62865176165773</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>175</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>None of the above</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>25-34</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>47.3873282528331</v>
+      </c>
+      <c r="E42" t="n">
+        <v>14.4115069221383</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-32.9758213306948</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>175</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>None of the above</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>35-44</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>47.3873282528331</v>
+      </c>
+      <c r="E43" t="n">
+        <v>14.9632323861088</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-32.4240958667243</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>322</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>67.56126614320391</v>
+      </c>
+      <c r="E44" t="n">
+        <v>42.1629520572403</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-25.3983140859636</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>323</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>31.2044505770528</v>
+      </c>
+      <c r="E45" t="n">
+        <v>57.8370479427597</v>
+      </c>
+      <c r="F45" t="n">
+        <v>26.6325973657069</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>346</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>45.5366680290527</v>
+      </c>
+      <c r="E46" t="n">
+        <v>76.502308525907</v>
+      </c>
+      <c r="F46" t="n">
+        <v>30.9656404968543</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>346</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>45.5366680290527</v>
+      </c>
+      <c r="E47" t="n">
+        <v>19.4592373378832</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-26.0774306911695</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>347</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>51.839294428448</v>
+      </c>
+      <c r="E48" t="n">
+        <v>20.3110967006958</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-31.5281977277522</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>347</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>51.839294428448</v>
+      </c>
+      <c r="E49" t="n">
+        <v>77.5125212514974</v>
+      </c>
+      <c r="F49" t="n">
+        <v>25.6732268230494</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>364</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>55.2343276522377</v>
+      </c>
+      <c r="E50" t="n">
+        <v>82.09633175914351</v>
+      </c>
+      <c r="F50" t="n">
+        <v>26.8620041069058</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>364</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>55.2343276522377</v>
+      </c>
+      <c r="E51" t="n">
+        <v>29.9667841614415</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-25.2675434907962</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>365</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>43.14710931796751</v>
+      </c>
+      <c r="E52" t="n">
+        <v>15.3114121561858</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-27.8356971617817</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>365</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>43.14710931796751</v>
+      </c>
+      <c r="E53" t="n">
+        <v>68.6920299503102</v>
+      </c>
+      <c r="F53" t="n">
+        <v>25.54492063234269</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>371</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>76.84270360258671</v>
+      </c>
+      <c r="E54" t="n">
+        <v>50.876126449762</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-25.9665771528247</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>382</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>38.5557273012625</v>
+      </c>
+      <c r="E55" t="n">
+        <v>72.924459523347</v>
+      </c>
+      <c r="F55" t="n">
+        <v>34.3687322220845</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>382</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>25-34</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>38.5557273012625</v>
+      </c>
+      <c r="E56" t="n">
+        <v>65.58350942006081</v>
+      </c>
+      <c r="F56" t="n">
+        <v>27.02778211879831</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>382</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>38.5557273012625</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2.76395011520717</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-35.79177718605533</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>383</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>59.48293426143911</v>
+      </c>
+      <c r="E58" t="n">
+        <v>23.8963569853921</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-35.586577276047</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>383</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>25-34</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>59.48293426143911</v>
+      </c>
+      <c r="E59" t="n">
+        <v>32.540606552569</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-26.9423277088701</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>383</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>59.48293426143911</v>
+      </c>
+      <c r="E60" t="n">
+        <v>95.27172331408291</v>
+      </c>
+      <c r="F60" t="n">
+        <v>35.7887890526438</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>394</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Have used Google Search to learn about this</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>36.3750119370025</v>
+      </c>
+      <c r="E61" t="n">
+        <v>6.229647870898971</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-30.14536406610353</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>395</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Have not used Google Search to learn about this</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>61.5343752734726</v>
+      </c>
+      <c r="E62" t="n">
+        <v>91.9919532146891</v>
+      </c>
+      <c r="F62" t="n">
+        <v>30.45757794121651</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>400</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Have used Google Search to learn about this</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>29.3175301556273</v>
+      </c>
+      <c r="E63" t="n">
+        <v>2.23361351778874</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-27.08391663783856</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>401</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Have not used Google Search to learn about this</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>67.95266581295351</v>
+      </c>
+      <c r="E64" t="n">
+        <v>97.7663864822113</v>
+      </c>
+      <c r="F64" t="n">
+        <v>29.81372066925779</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>406</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Have used Google Search to learn about this</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>50.95363275360339</v>
+      </c>
+      <c r="E65" t="n">
+        <v>18.9806235335705</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-31.97300922003289</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>407</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Have not used Google Search to learn about this</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>47.1738006755988</v>
+      </c>
+      <c r="E66" t="n">
+        <v>79.2409775520176</v>
+      </c>
+      <c r="F66" t="n">
+        <v>32.0671768764188</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>413</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Have not used Google Search to learn about this</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>73.96191855119289</v>
+      </c>
+      <c r="E67" t="n">
+        <v>48.2465004032729</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-25.71541814791999</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>418</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Have used Google Search to learn about this</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>25.2933930195299</v>
+      </c>
+      <c r="E68" t="n">
+        <v>56.9457528586307</v>
+      </c>
+      <c r="F68" t="n">
+        <v>31.65235983910081</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>419</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Have not used Google Search to learn about this</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>73.15486374910481</v>
+      </c>
+      <c r="E69" t="n">
+        <v>40.209233410972</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-32.9456303381328</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>496</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>I use Google Search primarily in my personal time</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>65.9632067798872</v>
+      </c>
+      <c r="E70" t="n">
+        <v>36.5507718784331</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-29.41243490145409</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>496</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>I use Google Search primarily in my personal time</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>65.9632067798872</v>
+      </c>
+      <c r="E71" t="n">
+        <v>95.12995079459769</v>
+      </c>
+      <c r="F71" t="n">
+        <v>29.1667440147105</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>563</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>71.8652305521771</v>
+      </c>
+      <c r="E72" t="n">
+        <v>46.7547251019557</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-25.11050545022139</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>564</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>27.0245347655942</v>
+      </c>
+      <c r="E73" t="n">
+        <v>53.2452748980443</v>
+      </c>
+      <c r="F73" t="n">
+        <v>26.2207401324501</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>570</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>54.70030349054979</v>
+      </c>
+      <c r="E74" t="n">
+        <v>79.9408803611381</v>
+      </c>
+      <c r="F74" t="n">
+        <v>25.24057687058831</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>581</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>34.5469270881924</v>
+      </c>
+      <c r="E75" t="n">
+        <v>60.6753005598083</v>
+      </c>
+      <c r="F75" t="n">
+        <v>26.1283734716159</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>581</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Have done this</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>34.5469270881924</v>
+      </c>
+      <c r="E76" t="n">
+        <v>7.5183365791529</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-27.0285905090395</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>582</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>63.7182978824977</v>
+      </c>
+      <c r="E77" t="n">
+        <v>37.2557272855678</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-26.4625705969299</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>582</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Have not done this</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>63.7182978824977</v>
+      </c>
+      <c r="E78" t="n">
+        <v>92.0061179168664</v>
+      </c>
+      <c r="F78" t="n">
+        <v>28.2878200343687</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>842</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Very helpful</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>47.0505299321654</v>
+      </c>
+      <c r="E79" t="n">
+        <v>75.2177694302668</v>
+      </c>
+      <c r="F79" t="n">
+        <v>28.1672394981014</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>843</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Somewhat helpful</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>46.7801420796451</v>
+      </c>
+      <c r="E80" t="n">
+        <v>8.136933550452879</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-38.64320852919222</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>866</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Very helpful</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>55-64</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>39.1376222358867</v>
+      </c>
+      <c r="E81" t="n">
+        <v>6.99032128675844</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-32.14730094912826</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>866</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Very helpful</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Northern Ireland</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>39.1376222358867</v>
+      </c>
+      <c r="E82" t="n">
+        <v>68.2458104988776</v>
+      </c>
+      <c r="F82" t="n">
+        <v>29.1081882629909</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>867</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Somewhat helpful</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>55-64</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>53.7859955887084</v>
+      </c>
+      <c r="E83" t="n">
+        <v>85.56776597523759</v>
+      </c>
+      <c r="F83" t="n">
+        <v>31.7817703865292</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>874</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Very helpful</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Northern Ireland</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>44.6602206631763</v>
+      </c>
+      <c r="E84" t="n">
+        <v>73.6950734583925</v>
+      </c>
+      <c r="F84" t="n">
+        <v>29.0348527952162</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>946</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>None of the above</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>18-24</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>63.9493798985966</v>
+      </c>
+      <c r="E85" t="n">
+        <v>35.6407734689511</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-28.3086064296455</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>946</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>None of the above</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>63.9493798985966</v>
+      </c>
+      <c r="E86" t="n">
+        <v>89.62262066557</v>
+      </c>
+      <c r="F86" t="n">
+        <v>25.67324076697339</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>968</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Essential - could not have earned the income without them</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>16.4124802258891</v>
+      </c>
+      <c r="E87" t="n">
+        <v>42.7993191945</v>
+      </c>
+      <c r="F87" t="n">
+        <v>26.3868389686109</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>968</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Essential - could not have earned the income without them</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Northern Ireland</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>16.4124802258891</v>
+      </c>
+      <c r="E88" t="n">
+        <v>52.97226648096331</v>
+      </c>
+      <c r="F88" t="n">
+        <v>36.5597862550742</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>1044</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Not true in my experience</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>55-64</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>51.0496003806399</v>
+      </c>
+      <c r="E89" t="n">
+        <v>86.2920425021081</v>
+      </c>
+      <c r="F89" t="n">
+        <v>35.2424421214682</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>1044</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Not true in my experience</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>51.0496003806399</v>
+      </c>
+      <c r="E90" t="n">
+        <v>78.74009035636369</v>
+      </c>
+      <c r="F90" t="n">
+        <v>27.6904899757238</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>1062</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Setting screen time limits</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>North West</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>52.5729245716356</v>
+      </c>
+      <c r="E91" t="n">
+        <v>92.07015319045711</v>
+      </c>
+      <c r="F91" t="n">
+        <v>39.4972286188215</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>1063</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Keeping track of your child’s physical location</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>North East</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>46.9346761309252</v>
+      </c>
+      <c r="E92" t="n">
+        <v>76.9381176512088</v>
+      </c>
+      <c r="F92" t="n">
+        <v>30.0034415202836</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>1063</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Keeping track of your child’s physical location</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Scotland</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>46.9346761309252</v>
+      </c>
+      <c r="E93" t="n">
+        <v>75.55106017693581</v>
+      </c>
+      <c r="F93" t="n">
+        <v>28.6163840460106</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>1077</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Would have been impossible</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>20.8014307786967</v>
+      </c>
+      <c r="E94" t="n">
+        <v>52.9661713823132</v>
+      </c>
+      <c r="F94" t="n">
+        <v>32.1647406036165</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>1078</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
           <t>Significantly more difficult</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>South East</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>47.2210113219907</v>
+      </c>
+      <c r="E95" t="n">
+        <v>72.74949838787509</v>
+      </c>
+      <c r="F95" t="n">
+        <v>25.5284870658844</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>1085</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Would have been impossible</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Northern Ireland</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>16.3265663416567</v>
+      </c>
+      <c r="E96" t="n">
+        <v>41.5629366769334</v>
+      </c>
+      <c r="F96" t="n">
+        <v>25.2363703352767</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>1086</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Significantly more difficult</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>West Midlands</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>49.1560149203012</v>
+      </c>
+      <c r="E97" t="n">
+        <v>20.8877130896868</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-28.2683018306144</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>1086</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Significantly more difficult</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Yorkshire and the Humber</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>49.1560149203012</v>
+      </c>
+      <c r="E98" t="n">
+        <v>75.6736190628945</v>
+      </c>
+      <c r="F98" t="n">
+        <v>26.5176041425933</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>1086</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Significantly more difficult</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>49.1560149203012</v>
+      </c>
+      <c r="E99" t="n">
+        <v>22.3909293651773</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-26.7650855551239</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>1087</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Somewhat more difficult</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>25.7372170148127</v>
+      </c>
+      <c r="E100" t="n">
+        <v>77.6090706348227</v>
+      </c>
+      <c r="F100" t="n">
+        <v>51.87185362000999</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>1088</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Would not have made much difference</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>35-44</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>8.169964514875131</v>
+      </c>
+      <c r="E101" t="n">
+        <v>49.505442985824</v>
+      </c>
+      <c r="F101" t="n">
+        <v>41.33547847094887</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>1088</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Would not have made much difference</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>45-54</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>8.169964514875131</v>
+      </c>
+      <c r="E102" t="n">
+        <v>59.1162973399879</v>
+      </c>
+      <c r="F102" t="n">
+        <v>50.94633282511277</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>1095</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Somewhat more difficult</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>North East</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>31.0616427222021</v>
+      </c>
+      <c r="E103" t="n">
+        <v>64.15589801476659</v>
+      </c>
+      <c r="F103" t="n">
+        <v>33.0942552925645</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>1102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Significantly more difficult</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
         <is>
           <t>East of England</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="D104" t="n">
         <v>35.4535835172556</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E104" t="n">
         <v>85.3524049118576</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F104" t="n">
         <v>49.898821394602</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>1102</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Significantly more difficult</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>North East</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>35.4535835172556</v>
+      </c>
+      <c r="E105" t="n">
+        <v>68.88823940626691</v>
+      </c>
+      <c r="F105" t="n">
+        <v>33.4346558890113</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>1104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Would not have made much difference</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>15.9374007538138</v>
+      </c>
+      <c r="E106" t="n">
+        <v>50</v>
+      </c>
+      <c r="F106" t="n">
+        <v>34.0625992461862</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>1180</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>I would keep access to Google Search</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>East Midlands</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>62.0496854628319</v>
+      </c>
+      <c r="E107" t="n">
+        <v>88.221873250044</v>
+      </c>
+      <c r="F107" t="n">
+        <v>26.1721877872121</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>1197</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>I would give up access to Google Search and get paid £50</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Northern Ireland</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>44.4355988063209</v>
+      </c>
+      <c r="E108" t="n">
+        <v>83.0961673701961</v>
+      </c>
+      <c r="F108" t="n">
+        <v>38.6605685638752</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>1245</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>I would give up access to all search engines and get paid £10</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Northern Ireland</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>23.8418854459486</v>
+      </c>
+      <c r="E109" t="n">
+        <v>52.482744964827</v>
+      </c>
+      <c r="F109" t="n">
+        <v>28.6408595188784</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>1257</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>I would give up access to all search engines and get paid £50</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>North East</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>34.965491398072</v>
+      </c>
+      <c r="E110" t="n">
+        <v>9.88270058274899</v>
+      </c>
+      <c r="F110" t="n">
+        <v>-25.08279081532301</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>1258</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>I would keep access to search engines</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Wales</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>53.2819222372675</v>
+      </c>
+      <c r="E111" t="n">
+        <v>27.1304713232312</v>
+      </c>
+      <c r="F111" t="n">
+        <v>-26.1514509140363</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>1275</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>I would give up access to all search engines and get paid £500</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Northern Ireland</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>54.2075674228092</v>
+      </c>
+      <c r="E112" t="n">
+        <v>88.72873193944871</v>
+      </c>
+      <c r="F112" t="n">
+        <v>34.5211645166395</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>1291</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Would take a fair amount longer (25% to 50% more time)</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>65+</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>32.0508999578288</v>
+      </c>
+      <c r="E113" t="n">
+        <v>7.005394036607</v>
+      </c>
+      <c r="F113" t="n">
+        <v>-25.0455059212218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>